<commit_message>
try fix some bugs
</commit_message>
<xml_diff>
--- a/Aluguel/stream-dash/df_recall.xlsx
+++ b/Aluguel/stream-dash/df_recall.xlsx
@@ -516,7 +516,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>44608</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>44608</v>
@@ -632,7 +632,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>44608</v>
@@ -690,7 +690,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>44608</v>
@@ -748,7 +748,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>44608</v>
@@ -806,7 +806,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>44608</v>
@@ -864,7 +864,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>44608</v>
@@ -1038,7 +1038,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>44608</v>
@@ -1154,7 +1154,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>44608</v>
@@ -1212,7 +1212,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B14" s="2" t="n">
         <v>44608</v>
@@ -1328,7 +1328,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>44608</v>
@@ -1386,7 +1386,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>44608</v>
@@ -1444,7 +1444,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="B18" s="2" t="n">
         <v>44608</v>
@@ -1502,7 +1502,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="B19" s="2" t="n">
         <v>44608</v>
@@ -1618,7 +1618,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="B21" s="2" t="n">
         <v>44608</v>
@@ -1734,7 +1734,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="B23" s="2" t="n">
         <v>44608</v>
@@ -1792,7 +1792,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="B24" s="2" t="n">
         <v>44608</v>
@@ -1850,7 +1850,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="B25" s="2" t="n">
         <v>44608</v>
@@ -1908,7 +1908,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="B26" s="2" t="n">
         <v>44608</v>
@@ -1966,7 +1966,7 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B27" s="2" t="n">
         <v>44608</v>
@@ -2604,7 +2604,7 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="B38" s="2" t="n">
         <v>44608</v>
@@ -2662,7 +2662,7 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="B39" s="2" t="n">
         <v>44608</v>
@@ -2720,7 +2720,7 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="B40" s="2" t="n">
         <v>44608</v>
@@ -2778,7 +2778,7 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B41" s="2" t="n">
         <v>44608</v>
@@ -2836,7 +2836,7 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="B42" s="2" t="n">
         <v>44608</v>
@@ -2894,7 +2894,7 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="B43" s="2" t="n">
         <v>44608</v>
@@ -2952,7 +2952,7 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="B44" s="2" t="n">
         <v>44608</v>
@@ -3010,7 +3010,7 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="B45" s="2" t="n">
         <v>44608</v>
@@ -3184,7 +3184,7 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="B48" s="2" t="n">
         <v>44608</v>
@@ -3300,7 +3300,7 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B50" s="2" t="n">
         <v>44608</v>
@@ -3358,7 +3358,7 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="B51" s="2" t="n">
         <v>44608</v>
@@ -3416,7 +3416,7 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="B52" s="2" t="n">
         <v>44608</v>
@@ -3590,7 +3590,7 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="B55" s="2" t="n">
         <v>44608</v>
@@ -3880,7 +3880,7 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="B60" s="2" t="n">
         <v>44608</v>
@@ -4112,7 +4112,7 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="B64" s="2" t="n">
         <v>44608</v>
@@ -4228,7 +4228,7 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="B66" s="2" t="n">
         <v>44608</v>
@@ -4344,7 +4344,7 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="B68" s="2" t="n">
         <v>44608</v>
@@ -5098,7 +5098,7 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="B81" s="2" t="n">
         <v>44608</v>
@@ -5214,7 +5214,7 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="B83" s="2" t="n">
         <v>44608</v>
@@ -5272,7 +5272,7 @@
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="B84" s="2" t="n">
         <v>44608</v>
@@ -5330,7 +5330,7 @@
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="B85" s="2" t="n">
         <v>44608</v>
@@ -5388,7 +5388,7 @@
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="B86" s="2" t="n">
         <v>44608</v>
@@ -5446,7 +5446,7 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="B87" s="2" t="n">
         <v>44608</v>
@@ -5504,7 +5504,7 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="B88" s="2" t="n">
         <v>44608</v>
@@ -5562,7 +5562,7 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="B89" s="2" t="n">
         <v>44608</v>
@@ -5620,7 +5620,7 @@
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B90" s="2" t="n">
         <v>44608</v>
@@ -5678,7 +5678,7 @@
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="B91" s="2" t="n">
         <v>44608</v>
@@ -5736,7 +5736,7 @@
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="B92" s="2" t="n">
         <v>44608</v>
@@ -5794,7 +5794,7 @@
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="B93" s="2" t="n">
         <v>44608</v>
@@ -5852,7 +5852,7 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="B94" s="2" t="n">
         <v>44608</v>
@@ -5910,7 +5910,7 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="B95" s="2" t="n">
         <v>44608</v>
@@ -5968,7 +5968,7 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="B96" s="2" t="n">
         <v>44608</v>
@@ -6026,7 +6026,7 @@
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="B97" s="2" t="n">
         <v>44608</v>
@@ -6084,7 +6084,7 @@
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="B98" s="2" t="n">
         <v>44608</v>
@@ -6142,7 +6142,7 @@
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="B99" s="2" t="n">
         <v>44608</v>
@@ -6200,7 +6200,7 @@
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B100" s="2" t="n">
         <v>44608</v>
@@ -6258,7 +6258,7 @@
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="B101" s="2" t="n">
         <v>44608</v>
@@ -6316,7 +6316,7 @@
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="B102" s="2" t="n">
         <v>44608</v>
@@ -6374,7 +6374,7 @@
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="B103" s="2" t="n">
         <v>44608</v>
@@ -6432,7 +6432,7 @@
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="B104" s="2" t="n">
         <v>44608</v>
@@ -6490,7 +6490,7 @@
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="B105" s="2" t="n">
         <v>44608</v>
@@ -6838,7 +6838,7 @@
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="B111" s="2" t="n">
         <v>44608</v>
@@ -7592,7 +7592,7 @@
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="B124" s="2" t="n">
         <v>44608</v>
@@ -7824,7 +7824,7 @@
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="B128" s="2" t="n">
         <v>44608</v>
@@ -8114,7 +8114,7 @@
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="B133" s="2" t="n">
         <v>44608</v>
@@ -8172,7 +8172,7 @@
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="B134" s="2" t="n">
         <v>44608</v>
@@ -8404,7 +8404,7 @@
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="B138" s="2" t="n">
         <v>44608</v>
@@ -8984,7 +8984,7 @@
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="B148" s="2" t="n">
         <v>44608</v>
@@ -9564,7 +9564,7 @@
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B158" s="2" t="n">
         <v>44608</v>
@@ -9970,7 +9970,7 @@
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="B165" s="2" t="n">
         <v>44608</v>
@@ -10028,7 +10028,7 @@
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="B166" s="2" t="n">
         <v>44608</v>
@@ -10086,7 +10086,7 @@
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="B167" s="2" t="n">
         <v>44608</v>
@@ -10144,7 +10144,7 @@
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="B168" s="2" t="n">
         <v>44608</v>
@@ -10434,7 +10434,7 @@
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="B173" s="2" t="n">
         <v>44608</v>
@@ -10492,7 +10492,7 @@
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="B174" s="2" t="n">
         <v>44608</v>
@@ -10608,7 +10608,7 @@
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="B176" s="2" t="n">
         <v>44608</v>
@@ -10666,7 +10666,7 @@
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="B177" s="2" t="n">
         <v>44608</v>
@@ -10840,7 +10840,7 @@
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="B180" s="2" t="n">
         <v>44608</v>
@@ -10898,7 +10898,7 @@
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="B181" s="2" t="n">
         <v>44608</v>
@@ -11420,7 +11420,7 @@
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="B190" s="2" t="n">
         <v>44608</v>
@@ -11594,7 +11594,7 @@
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="B193" s="2" t="n">
         <v>44608</v>
@@ -11652,7 +11652,7 @@
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="B194" s="2" t="n">
         <v>44608</v>
@@ -11710,7 +11710,7 @@
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="B195" s="2" t="n">
         <v>44608</v>
@@ -11768,7 +11768,7 @@
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="B196" s="2" t="n">
         <v>44608</v>
@@ -11826,7 +11826,7 @@
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="B197" s="2" t="n">
         <v>44608</v>
@@ -12116,7 +12116,7 @@
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="B202" s="2" t="n">
         <v>44608</v>
@@ -12174,7 +12174,7 @@
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="B203" s="2" t="n">
         <v>44608</v>
@@ -12232,7 +12232,7 @@
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="B204" s="2" t="n">
         <v>44608</v>
@@ -12290,7 +12290,7 @@
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="B205" s="2" t="n">
         <v>44608</v>
@@ -12348,7 +12348,7 @@
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B206" s="2" t="n">
         <v>44608</v>
@@ -12406,7 +12406,7 @@
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="B207" s="2" t="n">
         <v>44608</v>
@@ -12638,7 +12638,7 @@
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="B211" s="2" t="n">
         <v>44608</v>
@@ -12812,7 +12812,7 @@
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="B214" s="2" t="n">
         <v>44608</v>
@@ -12870,7 +12870,7 @@
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="B215" s="2" t="n">
         <v>44608</v>
@@ -12928,7 +12928,7 @@
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="B216" s="2" t="n">
         <v>44608</v>
@@ -12986,7 +12986,7 @@
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="B217" s="2" t="n">
         <v>44608</v>
@@ -13334,7 +13334,7 @@
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="B223" s="2" t="n">
         <v>44608</v>
@@ -13392,7 +13392,7 @@
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="B224" s="2" t="n">
         <v>44608</v>
@@ -13798,7 +13798,7 @@
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="B231" s="2" t="n">
         <v>44608</v>
@@ -13856,7 +13856,7 @@
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="B232" s="2" t="n">
         <v>44608</v>
@@ -13914,7 +13914,7 @@
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="B233" s="2" t="n">
         <v>44608</v>
@@ -14030,7 +14030,7 @@
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="B235" s="2" t="n">
         <v>44608</v>
@@ -14088,7 +14088,7 @@
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="B236" s="2" t="n">
         <v>44608</v>
@@ -14146,7 +14146,7 @@
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B237" s="2" t="n">
         <v>44608</v>
@@ -14204,7 +14204,7 @@
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="B238" s="2" t="n">
         <v>44608</v>
@@ -14262,7 +14262,7 @@
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="B239" s="2" t="n">
         <v>44608</v>
@@ -14378,7 +14378,7 @@
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B241" s="2" t="n">
         <v>44608</v>
@@ -14494,7 +14494,7 @@
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="B243" s="2" t="n">
         <v>44608</v>
@@ -14552,7 +14552,7 @@
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="B244" s="2" t="n">
         <v>44608</v>
@@ -14610,7 +14610,7 @@
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="B245" s="2" t="n">
         <v>44608</v>
@@ -14668,7 +14668,7 @@
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B246" s="2" t="n">
         <v>44608</v>
@@ -14726,7 +14726,7 @@
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="B247" s="2" t="n">
         <v>44608</v>
@@ -14784,7 +14784,7 @@
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="B248" s="2" t="n">
         <v>44608</v>
@@ -14842,7 +14842,7 @@
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="B249" s="2" t="n">
         <v>44608</v>
@@ -14900,7 +14900,7 @@
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="B250" s="2" t="n">
         <v>44608</v>
@@ -15016,7 +15016,7 @@
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="B252" s="2" t="n">
         <v>44608</v>
@@ -15074,7 +15074,7 @@
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="B253" s="2" t="n">
         <v>44608</v>
@@ -15422,7 +15422,7 @@
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="B259" s="2" t="n">
         <v>44608</v>
@@ -15480,7 +15480,7 @@
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B260" s="2" t="n">
         <v>44608</v>
@@ -15712,7 +15712,7 @@
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="B264" s="2" t="n">
         <v>44608</v>
@@ -15886,7 +15886,7 @@
     </row>
     <row r="267">
       <c r="A267" s="1" t="n">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B267" s="2" t="n">
         <v>44608</v>
@@ -15944,7 +15944,7 @@
     </row>
     <row r="268">
       <c r="A268" s="1" t="n">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B268" s="2" t="n">
         <v>44608</v>
@@ -16002,7 +16002,7 @@
     </row>
     <row r="269">
       <c r="A269" s="1" t="n">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="B269" s="2" t="n">
         <v>44608</v>
@@ -16640,7 +16640,7 @@
     </row>
     <row r="280">
       <c r="A280" s="1" t="n">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="B280" s="2" t="n">
         <v>44608</v>
@@ -17800,7 +17800,7 @@
     </row>
     <row r="300">
       <c r="A300" s="1" t="n">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="B300" s="2" t="n">
         <v>44608</v>
@@ -17858,7 +17858,7 @@
     </row>
     <row r="301">
       <c r="A301" s="1" t="n">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="B301" s="2" t="n">
         <v>44608</v>
@@ -17916,7 +17916,7 @@
     </row>
     <row r="302">
       <c r="A302" s="1" t="n">
-        <v>1068</v>
+        <v>102</v>
       </c>
       <c r="B302" s="2" t="n">
         <v>44608</v>
@@ -17951,7 +17951,7 @@
         <v>-5830</v>
       </c>
       <c r="J302" t="n">
-        <v>-0</v>
+        <v>5830</v>
       </c>
       <c r="K302" t="n">
         <v>0</v>

</xml_diff>